<commit_message>
new changes with extended report
</commit_message>
<xml_diff>
--- a/crmSeleniumProject/data/testData.xlsx
+++ b/crmSeleniumProject/data/testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14700" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15330" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -94,24 +94,9 @@
     <t>1may_2_b20</t>
   </si>
   <si>
-    <t>16swati10</t>
-  </si>
-  <si>
-    <t>26swati30</t>
-  </si>
-  <si>
-    <t>36swati20</t>
-  </si>
-  <si>
     <t>16sahil2</t>
   </si>
   <si>
-    <t>16hdfc15</t>
-  </si>
-  <si>
-    <t>36hdfc16</t>
-  </si>
-  <si>
     <t>46hdfc34</t>
   </si>
   <si>
@@ -137,6 +122,21 @@
   </si>
   <si>
     <t>19newspaper20</t>
+  </si>
+  <si>
+    <t>16hdfc16</t>
+  </si>
+  <si>
+    <t>16swati19</t>
+  </si>
+  <si>
+    <t>26swati39</t>
+  </si>
+  <si>
+    <t>36swati29</t>
+  </si>
+  <si>
+    <t>36hdfc20</t>
   </si>
 </sst>
 </file>
@@ -478,7 +478,7 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,16 +526,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>4</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
         <v>24</v>
@@ -549,7 +549,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
         <v>19</v>
@@ -563,10 +563,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -602,13 +602,13 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I7" t="s">
         <v>33</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -619,16 +619,16 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" t="s">
         <v>34</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>